<commit_message>
Example of a codebook
</commit_message>
<xml_diff>
--- a/data_harmonization/examples/data-harmonization-1/codebook_example.xlsx
+++ b/data_harmonization/examples/data-harmonization-1/codebook_example.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Projects/memorabel/data_harmonization/examples/data-harmonization-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAB9BFF-1E56-004C-9882-A68EF234F2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298F5E80-F1F9-3740-B253-0844F3560653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="2220" windowWidth="27640" windowHeight="16940" xr2:uid="{4F26F78B-1925-3045-B73D-09D96D3A169A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="16940" activeTab="1" xr2:uid="{4F26F78B-1925-3045-B73D-09D96D3A169A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="codebook" sheetId="1" r:id="rId1"/>
+    <sheet name="mapping" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="289">
   <si>
     <t>Variable</t>
   </si>
@@ -211,13 +212,732 @@
   </si>
   <si>
     <t>type 1.0 or 2.0</t>
+  </si>
+  <si>
+    <t>Variable name used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable Description </t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Variable name</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Way of measurement/definition</t>
+  </si>
+  <si>
+    <t>FU available? If yes, please specify name FU measurements and provide FU dates</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Data_saved</t>
+  </si>
+  <si>
+    <t>CSV/excel/SPSS/SAS/R/Phyton/other</t>
+  </si>
+  <si>
+    <t>Format_data</t>
+  </si>
+  <si>
+    <t>In long or in wide format</t>
+  </si>
+  <si>
+    <t>Long or wide format: wide</t>
+  </si>
+  <si>
+    <t>In wide format, all variable names get a suffix t0, t1, t2 etc for measurement wave</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Participant ID</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>Birth_year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year of birth </t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age at assessment </t>
+  </si>
+  <si>
+    <t>age in years</t>
+  </si>
+  <si>
+    <t>Education_years</t>
+  </si>
+  <si>
+    <t>Education level in years</t>
+  </si>
+  <si>
+    <t>Education_category</t>
+  </si>
+  <si>
+    <t>Education level categories</t>
+  </si>
+  <si>
+    <t>1 = primary school
+2 = lower vocational education
+3 = intermediate secondary education
+4 = intermediate vocational education
+5 = general secondary education, up to third year
+6 = general secondary education, completed
+7 = higher vocational education
+8 = university candidate degree
+9 = university completed</t>
+  </si>
+  <si>
+    <t>Dementia</t>
+  </si>
+  <si>
+    <t>Date_diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of diagnosis </t>
+  </si>
+  <si>
+    <t>Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnosis </t>
+  </si>
+  <si>
+    <t>Please provide definitions used for classification</t>
+  </si>
+  <si>
+    <t>Date_CDR</t>
+  </si>
+  <si>
+    <t>Date Clinical Dementia Rating Scale assessment</t>
+  </si>
+  <si>
+    <t>CDR_total</t>
+  </si>
+  <si>
+    <t>Clinical Dementia Rating total score</t>
+  </si>
+  <si>
+    <t>Mortality</t>
+  </si>
+  <si>
+    <t>Mort_Date</t>
+  </si>
+  <si>
+    <t>Date of death</t>
+  </si>
+  <si>
+    <t>Live_Date</t>
+  </si>
+  <si>
+    <t>Last known date to be alive</t>
+  </si>
+  <si>
+    <t>Mort</t>
+  </si>
+  <si>
+    <t>Cardiovascular</t>
+  </si>
+  <si>
+    <t>Please include all available dates for different types of cardiovascular assessments, even if not listed here</t>
+  </si>
+  <si>
+    <t>Date_vitals</t>
+  </si>
+  <si>
+    <t>Date assessment vital signs</t>
+  </si>
+  <si>
+    <t>SBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systolic blood pressure </t>
+  </si>
+  <si>
+    <t>DBP</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>BMI: weight/(bodylength_cm/100)^2)</t>
+  </si>
+  <si>
+    <t>kg/m2</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height </t>
+  </si>
+  <si>
+    <t>Date_comorbidities</t>
+  </si>
+  <si>
+    <t>Date assessment comorbidities</t>
+  </si>
+  <si>
+    <t>If medication use and  comorbidities were assessed on different dates, please specify names of both variables</t>
+  </si>
+  <si>
+    <t>Hypertension</t>
+  </si>
+  <si>
+    <t>History of hypertension yes/no</t>
+  </si>
+  <si>
+    <t>Please indicate how history of hypertension was defined</t>
+  </si>
+  <si>
+    <t>0 = no hypertension; 1 = hypertension</t>
+  </si>
+  <si>
+    <t>SBP &gt;= 90 or DPB &gt;= 140</t>
+  </si>
+  <si>
+    <t>History of hypercholesterolemia yes/no</t>
+  </si>
+  <si>
+    <t>Please indicate how history of hypercholesterolemia  was defined</t>
+  </si>
+  <si>
+    <t>DM_1</t>
+  </si>
+  <si>
+    <t>Diabetes Mellitus type 1 yes/no</t>
+  </si>
+  <si>
+    <t>1 = yes; 2 = no</t>
+  </si>
+  <si>
+    <t>type not available</t>
+  </si>
+  <si>
+    <t>DM_2</t>
+  </si>
+  <si>
+    <t>Diabetes Mellitus type 2 yes/no</t>
+  </si>
+  <si>
+    <t>Myocardial_infarction</t>
+  </si>
+  <si>
+    <t>Myocardial infarction yes/no</t>
+  </si>
+  <si>
+    <t>Heart_failure</t>
+  </si>
+  <si>
+    <t>Heart failure yes/no</t>
+  </si>
+  <si>
+    <t>Stroke</t>
+  </si>
+  <si>
+    <t>Stroke yes/no</t>
+  </si>
+  <si>
+    <t>Drugs_hypertension</t>
+  </si>
+  <si>
+    <t>Anti-hypertensive drugs</t>
+  </si>
+  <si>
+    <t>Drugs_hypercholesterolemia</t>
+  </si>
+  <si>
+    <t>Hypercholesterolemia medication</t>
+  </si>
+  <si>
+    <t>Drugs_diabetes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diabetes Mellitus type 2 medication </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info </t>
+  </si>
+  <si>
+    <t>Date_blood</t>
+  </si>
+  <si>
+    <t>Date blood collection</t>
+  </si>
+  <si>
+    <t>If glucose and cholesterol were assessed on different dates, please specify names of both variables</t>
+  </si>
+  <si>
+    <t>Glucose_fasted</t>
+  </si>
+  <si>
+    <t>Fasted glucose blood</t>
+  </si>
+  <si>
+    <t>Glucose_nonfasted</t>
+  </si>
+  <si>
+    <t>Non-fasted glucose blood</t>
+  </si>
+  <si>
+    <t>Glucose_abnormal</t>
+  </si>
+  <si>
+    <t>Glucose dichotomized into normal/abnormal</t>
+  </si>
+  <si>
+    <t>Glucose_cutoff</t>
+  </si>
+  <si>
+    <t>Cutoff used for dichotemization glucose</t>
+  </si>
+  <si>
+    <t>Cutoff used:</t>
+  </si>
+  <si>
+    <t>High density lipoprotein cholesterol blood</t>
+  </si>
+  <si>
+    <t>mmol/L</t>
+  </si>
+  <si>
+    <t>Low density lipoprotein cholesterol blood</t>
+  </si>
+  <si>
+    <t>CRP</t>
+  </si>
+  <si>
+    <t>C-reactive protein</t>
+  </si>
+  <si>
+    <t>Date_habits</t>
+  </si>
+  <si>
+    <t>Date assessment alcohol and smoking habits</t>
+  </si>
+  <si>
+    <t>Alcohol</t>
+  </si>
+  <si>
+    <t>Current alcohol use yes/no</t>
+  </si>
+  <si>
+    <t>Units of alcohol per day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current/past / never smoking </t>
+  </si>
+  <si>
+    <t>Current/never if information on past smoking (=&lt; 10 years ago) is not available</t>
+  </si>
+  <si>
+    <t>rook3cat</t>
+  </si>
+  <si>
+    <t>APOE_Date</t>
+  </si>
+  <si>
+    <t>Date of assessment APOE</t>
+  </si>
+  <si>
+    <t>APOE_carrier</t>
+  </si>
+  <si>
+    <t>APOE e4 carrier yes/no</t>
+  </si>
+  <si>
+    <t>0 = non-carrier; 1 = heterozygote; 2= homozygote</t>
+  </si>
+  <si>
+    <t>APOE_genotype</t>
+  </si>
+  <si>
+    <t>E2/E2, E2/E3, E6/E3, E3/E4, E4/E4, E2/E4</t>
+  </si>
+  <si>
+    <t>E3/E3 was renamed to E6/E3 for convenience</t>
+  </si>
+  <si>
+    <t>Amyloid/(P)Tau</t>
+  </si>
+  <si>
+    <t>Date_LP</t>
+  </si>
+  <si>
+    <t>Date lumbar puncture</t>
+  </si>
+  <si>
+    <t>CSF_assay_amyloid</t>
+  </si>
+  <si>
+    <t>CSF Assay Amyloid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assay used: </t>
+  </si>
+  <si>
+    <t>CSF_ab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amyloid beta in CSF </t>
+  </si>
+  <si>
+    <t>Priority for 1. Amyloid Beta 1-42 in pg/ml                                                    2. Ratio Amyloid Beta 42/40                                                                                  3. Amyloid Beta 1-38 in pg/ml</t>
+  </si>
+  <si>
+    <t>Amy_abnormal</t>
+  </si>
+  <si>
+    <t>Amyloid beta dichotomised</t>
+  </si>
+  <si>
+    <t>Amy_cutoff</t>
+  </si>
+  <si>
+    <t>Cutoff used for amyloid dichotemization</t>
+  </si>
+  <si>
+    <t>Please indicate which cut-off was used in your cohort</t>
+  </si>
+  <si>
+    <t>CSF_assay_Tau</t>
+  </si>
+  <si>
+    <t>CSF Assay tau</t>
+  </si>
+  <si>
+    <t>CSF_ttau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Tau </t>
+  </si>
+  <si>
+    <t>Ttau_abnormal</t>
+  </si>
+  <si>
+    <t>Total Tau dichotomised</t>
+  </si>
+  <si>
+    <t>Ttau_cutoff</t>
+  </si>
+  <si>
+    <t>Cutoff used for total tau dichotemization</t>
+  </si>
+  <si>
+    <t>CSF_ptau</t>
+  </si>
+  <si>
+    <t>Phosphorylated Tau</t>
+  </si>
+  <si>
+    <t>Ptau_abnormal</t>
+  </si>
+  <si>
+    <t>Phosphorylated Tau dichotemised</t>
+  </si>
+  <si>
+    <t>Ptau_cutoff</t>
+  </si>
+  <si>
+    <t>Cutoff used for phosphorylated tau dichotemization</t>
+  </si>
+  <si>
+    <t>Date_PET</t>
+  </si>
+  <si>
+    <t>Date PET scan</t>
+  </si>
+  <si>
+    <t>PET_tracer</t>
+  </si>
+  <si>
+    <t>Tracer used during PET assessment</t>
+  </si>
+  <si>
+    <t>Tracer used:</t>
+  </si>
+  <si>
+    <t>PET_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method used to express amyloid uptake in PET </t>
+  </si>
+  <si>
+    <t>Method used:</t>
+  </si>
+  <si>
+    <t>Pet_assesment</t>
+  </si>
+  <si>
+    <t>Assessment of PET scan visual or quantitative</t>
+  </si>
+  <si>
+    <t>Visual or quantitative assessment:</t>
+  </si>
+  <si>
+    <t>PET_level</t>
+  </si>
+  <si>
+    <t>Result PET assessment, continuous</t>
+  </si>
+  <si>
+    <t>PET_abnormal</t>
+  </si>
+  <si>
+    <t>Amyloid positivity on PET yes/no</t>
+  </si>
+  <si>
+    <t>Anxiety/depression</t>
+  </si>
+  <si>
+    <t>Date_depression</t>
+  </si>
+  <si>
+    <t>Date assesment depression</t>
+  </si>
+  <si>
+    <t>Depression_rating / Depression</t>
+  </si>
+  <si>
+    <t>Result assessment depression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priority for 1. clinical diagnosis                                                                       2. MINI                                                                                                                             3. GDS-15                                                                                                                                4. GDS                                                                                                                           5. CES-D                                                                                                                             6. If not available, please provide alternative if possible   </t>
+  </si>
+  <si>
+    <t>Depression_cutoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cutoff used </t>
+  </si>
+  <si>
+    <t>If relevant, please  indicate which cut-off for the depression questionnaire has been used in your cohort</t>
+  </si>
+  <si>
+    <t>Date_anxiety</t>
+  </si>
+  <si>
+    <t>Date assessment anxiety</t>
+  </si>
+  <si>
+    <t>Anxiety_rating / Anxiety</t>
+  </si>
+  <si>
+    <t>Result assesment anxiety</t>
+  </si>
+  <si>
+    <t>Priority for 1. clinical diagnosis                                                                   2.  MINI                                                                                                                          3. Beck anxiety                                                                                                             4.  State-Trait anxiety inventory                                                                        5. Hospital anxiety and depresson scale                                                             6. If not available, please provide alternative if possible</t>
+  </si>
+  <si>
+    <t>Anxiety_cutoff</t>
+  </si>
+  <si>
+    <t>If relevant, please  indicate which cut-off for the anxiety questionnaire has been used in your cohort</t>
+  </si>
+  <si>
+    <t>Cognition</t>
+  </si>
+  <si>
+    <t>Date_MMSE</t>
+  </si>
+  <si>
+    <t>Date MMSE assessment</t>
+  </si>
+  <si>
+    <t>MMSE_total</t>
+  </si>
+  <si>
+    <t>MMSE total score</t>
+  </si>
+  <si>
+    <t>Date_NPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of neuropsychological examination </t>
+  </si>
+  <si>
+    <t>Priority_attention</t>
+  </si>
+  <si>
+    <t>raw score attention test</t>
+  </si>
+  <si>
+    <t>Priority for 1. Trail Making Test A 
+2. Stroop 1
+3. Stroop 2
+4. Symbol Digit Substitution Task                                                                         5.  If not available, please provide alternative if possible      Trail Making Test can be replaced by Concept Shifting Test</t>
+  </si>
+  <si>
+    <t>Priority_memory_im</t>
+  </si>
+  <si>
+    <t>raw score memory test immediate</t>
+  </si>
+  <si>
+    <t>Priority for 1. Ray Auditory Verbal Learning Test (RAVLT)
+2. CERAD
+3. Grober-Buschke FCSRT
+4. Story recall test
+5. Logical memory
+6. Hopkins
+7. VAT
+8. Story recall Brescia
+9. Recall Rey figure
+10. MMSE
+11. ADAS-Cog
+12. 10 word list
+13. immediate recall 10 word list                                                                    14. if not available, please provide alternative if possible</t>
+  </si>
+  <si>
+    <t>Priority_memory_dr</t>
+  </si>
+  <si>
+    <t>raw score memory test delayed</t>
+  </si>
+  <si>
+    <t>Priority_executive</t>
+  </si>
+  <si>
+    <t>raw score executive test</t>
+  </si>
+  <si>
+    <t>Priority for 1. Trail Making Test B
+2. Stroop 3                                                                                                                  3. if not available, please provide alternative if possible        Trail Making Test can be replaced by Concept Shifting Test</t>
+  </si>
+  <si>
+    <t>Priority_language</t>
+  </si>
+  <si>
+    <t>raw score language test</t>
+  </si>
+  <si>
+    <t>Priority for 1. Animal Fluency 1 min
+2. Category Fluency 1 min
+3. Letter Fluency 1 min
+4. Any type of fluency 2 min
+5. Boston Naming Test (15/30/60 items)
+6. Any picture naming test                                                                                 7. if not available, please provide alternative if possible</t>
+  </si>
+  <si>
+    <t>Plasma</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>P-Tau</t>
+  </si>
+  <si>
+    <t>P-Tau in plasma</t>
+  </si>
+  <si>
+    <t>Amyloid-B-42</t>
+  </si>
+  <si>
+    <t>Amyloid-B-42 in plasma</t>
+  </si>
+  <si>
+    <t>Amyloid-B_40</t>
+  </si>
+  <si>
+    <t>Amyloid-B_40 in plasma</t>
+  </si>
+  <si>
+    <t>GFAP</t>
+  </si>
+  <si>
+    <t>Glial Fibrillary acidic protein</t>
+  </si>
+  <si>
+    <t>NFL</t>
+  </si>
+  <si>
+    <t>Neurofilament light</t>
+  </si>
+  <si>
+    <t>E-Selectin</t>
+  </si>
+  <si>
+    <t>E-selectin (CD62E)</t>
+  </si>
+  <si>
+    <t>SAA</t>
+  </si>
+  <si>
+    <t>Serum Amyloid A</t>
+  </si>
+  <si>
+    <t>VCAM</t>
+  </si>
+  <si>
+    <t>Vascular cellular adhesion molecule</t>
+  </si>
+  <si>
+    <t>ICAM</t>
+  </si>
+  <si>
+    <t>Intercellular adhesion molecule</t>
+  </si>
+  <si>
+    <t>Il6</t>
+  </si>
+  <si>
+    <t>Interleukin-6</t>
+  </si>
+  <si>
+    <t>Il8</t>
+  </si>
+  <si>
+    <t>Interleukin-8</t>
+  </si>
+  <si>
+    <t>Il-1b</t>
+  </si>
+  <si>
+    <t>Interleukin 1 beta</t>
+  </si>
+  <si>
+    <t>TNFalpha</t>
+  </si>
+  <si>
+    <t>Tumor necrosis factor alpa</t>
+  </si>
+  <si>
+    <t>Format used: CSV</t>
+  </si>
+  <si>
+    <t>m = male; f = female</t>
+  </si>
+  <si>
+    <t>1 = alive, 2 = dead, 3 = unknown</t>
+  </si>
+  <si>
+    <t>dat_ms</t>
+  </si>
+  <si>
+    <t>1 = smoker; 2 = former smoker; 3 = never smoker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -233,8 +953,83 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,8 +1042,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7F7F7F"/>
+        <bgColor rgb="FF7F7F7F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8D8D8"/>
+        <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -256,13 +1081,211 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473A7F59-7440-BA46-AB1F-DB0CA08E94D6}">
   <dimension ref="B1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -871,4 +1894,1660 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C236F84-8DB9-0247-89DD-300B6AC1A01F}">
+  <dimension ref="A1:H107"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.1640625" customWidth="1"/>
+    <col min="2" max="2" width="50.1640625" customWidth="1"/>
+    <col min="3" max="3" width="55" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="5" max="5" width="39.5" customWidth="1"/>
+    <col min="6" max="6" width="37.5" customWidth="1"/>
+    <col min="7" max="7" width="50.5" customWidth="1"/>
+    <col min="8" max="8" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="21"/>
+      <c r="D20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="7"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="23"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="7"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="12"/>
+    </row>
+    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G48" s="6"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="30"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="23"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G52" s="6"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="C60" s="31"/>
+      <c r="D60" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="12"/>
+    </row>
+    <row r="61" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C62" s="22"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="12"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C64" s="22"/>
+      <c r="D64" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="12"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" s="22"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C66" s="22"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="12"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C68" s="22"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C69" s="22"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="12"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C71" s="22"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C72" s="22"/>
+      <c r="D72" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="12"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="12"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C74" s="9"/>
+      <c r="D74" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="12"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="7"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C78" s="33"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="7"/>
+    </row>
+    <row r="79" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A79" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C79" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="7"/>
+    </row>
+    <row r="80" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A80" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="D80" s="10"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="12"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="23"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="7"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C82" s="20"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="7"/>
+    </row>
+    <row r="83" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="A83" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C83" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="7"/>
+    </row>
+    <row r="84" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A84" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="12"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="7"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="B86" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="C86" s="22"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="7"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="C87" s="33"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="7"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C88" s="36"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="7"/>
+    </row>
+    <row r="89" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A89" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D89" s="6"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="7"/>
+    </row>
+    <row r="90" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+      <c r="A90" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B90" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="7"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C91" s="9"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="7"/>
+    </row>
+    <row r="92" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A92" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="7"/>
+    </row>
+    <row r="93" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+      <c r="A93" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="7"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="E94" s="38"/>
+      <c r="F94" s="38"/>
+      <c r="G94" s="38"/>
+      <c r="H94" s="39"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C95" s="22"/>
+      <c r="D95" s="40"/>
+      <c r="E95" s="40"/>
+      <c r="F95" s="40"/>
+      <c r="G95" s="40"/>
+      <c r="H95" s="41"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C96" s="9"/>
+      <c r="D96" s="40"/>
+      <c r="E96" s="40"/>
+      <c r="F96" s="40"/>
+      <c r="G96" s="40"/>
+      <c r="H96" s="41"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C97" s="9"/>
+      <c r="D97" s="40"/>
+      <c r="E97" s="40"/>
+      <c r="F97" s="40"/>
+      <c r="G97" s="40"/>
+      <c r="H97" s="41"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C98" s="9"/>
+      <c r="D98" s="40"/>
+      <c r="E98" s="40"/>
+      <c r="F98" s="40"/>
+      <c r="G98" s="40"/>
+      <c r="H98" s="41"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="C99" s="9"/>
+      <c r="D99" s="40"/>
+      <c r="E99" s="40"/>
+      <c r="F99" s="40"/>
+      <c r="G99" s="40"/>
+      <c r="H99" s="41"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C100" s="9"/>
+      <c r="D100" s="40"/>
+      <c r="E100" s="40"/>
+      <c r="F100" s="40"/>
+      <c r="G100" s="40"/>
+      <c r="H100" s="41"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C101" s="9"/>
+      <c r="D101" s="40"/>
+      <c r="E101" s="40"/>
+      <c r="F101" s="40"/>
+      <c r="G101" s="40"/>
+      <c r="H101" s="41"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C102" s="9"/>
+      <c r="D102" s="40"/>
+      <c r="E102" s="40"/>
+      <c r="F102" s="40"/>
+      <c r="G102" s="40"/>
+      <c r="H102" s="41"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="C103" s="9"/>
+      <c r="D103" s="40"/>
+      <c r="E103" s="40"/>
+      <c r="F103" s="40"/>
+      <c r="G103" s="40"/>
+      <c r="H103" s="41"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C104" s="9"/>
+      <c r="D104" s="40"/>
+      <c r="E104" s="40"/>
+      <c r="F104" s="40"/>
+      <c r="G104" s="40"/>
+      <c r="H104" s="41"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C105" s="9"/>
+      <c r="D105" s="40"/>
+      <c r="E105" s="40"/>
+      <c r="F105" s="40"/>
+      <c r="G105" s="40"/>
+      <c r="H105" s="41"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C106" s="9"/>
+      <c r="D106" s="40"/>
+      <c r="E106" s="40"/>
+      <c r="F106" s="40"/>
+      <c r="G106" s="40"/>
+      <c r="H106" s="41"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C107" s="9"/>
+      <c r="D107" s="40"/>
+      <c r="E107" s="40"/>
+      <c r="F107" s="40"/>
+      <c r="G107" s="40"/>
+      <c r="H107" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="D94:H94"/>
+    <mergeCell ref="D70:H70"/>
+    <mergeCell ref="D72:H72"/>
+    <mergeCell ref="D73:H73"/>
+    <mergeCell ref="D74:H74"/>
+    <mergeCell ref="D80:H80"/>
+    <mergeCell ref="D84:H84"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D46:H46"/>
+    <mergeCell ref="D60:H60"/>
+    <mergeCell ref="D63:H63"/>
+    <mergeCell ref="D64:H64"/>
+    <mergeCell ref="D67:H67"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>